<commit_message>
jn:actualizacion dicc 01 fecha
</commit_message>
<xml_diff>
--- a/05_Entregable 3/envio/Diccionarios/MD_01_Fiscalía_Informe_estadistico_2025012322001116 FIscalia.xlsx
+++ b/05_Entregable 3/envio/Diccionarios/MD_01_Fiscalía_Informe_estadistico_2025012322001116 FIscalia.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco_F\!!Personal\Mio\1_WCS 2024\wcs\05_Entregable 3\previo\Diccionarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Javi_Angelito\wcs\05_Entregable 3\envio\Diccionarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEA20D6-F482-4DD9-9C5F-F2DB7941A2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
@@ -355,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -739,11 +740,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +782,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>45721</v>
+        <v>45782</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -807,7 +808,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -891,10 +892,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="B6" sqref="B6"/>
       <selection pane="topRight" activeCell="B17" sqref="B17"/>
@@ -1368,10 +1369,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="G16:G18">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="G16:G18" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>-1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="G5:G6">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="G5:G6" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>